<commit_message>
Deploying to gh-pages from  @ 03a89f1f6cee893ef522429aebf9690c0e95d179 🚀
</commit_message>
<xml_diff>
--- a/2021-02-01.xlsx
+++ b/2021-02-01.xlsx
@@ -2,27 +2,22 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20368"/>
-  <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\Projekte\Abt3_IQM-COVID19\Fachlich\Auswertungen\2021-02-01\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36805F25-FE3D-401D-BF94-FC7A5C01629C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8CCB849-869D-4BA2-83B8-A937745B1C06}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="105" windowWidth="28515" windowHeight="12600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="120" yWindow="105" windowWidth="28515" windowHeight="12600" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Erläuterung" sheetId="9" r:id="rId1"/>
-    <sheet name="Gesamt_bis_einschl_31.01.21" sheetId="12" r:id="rId2"/>
-    <sheet name="Indik_bis_einschl_31.01." sheetId="11" r:id="rId3"/>
+    <sheet name="Gesamt_bis_einschl_01.02.21" sheetId="12" r:id="rId2"/>
+    <sheet name="Indik_bis_einschl_01.02." sheetId="11" r:id="rId3"/>
     <sheet name="Impfungen_proTag" sheetId="10" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="Bundesländer001" localSheetId="1">Gesamt_bis_einschl_31.01.21!#REF!</definedName>
-    <definedName name="Bundesländer001" localSheetId="2">Indik_bis_einschl_31.01.!$G$2:$J$18</definedName>
-    <definedName name="Bundesländer001_1" localSheetId="1">Gesamt_bis_einschl_31.01.21!$D$3:$G$19</definedName>
-    <definedName name="Bundesländer001_1" localSheetId="2">Indik_bis_einschl_31.01.!$C$2:$F$18</definedName>
+    <definedName name="Bundesländer001" localSheetId="1">Gesamt_bis_einschl_01.02.21!#REF!</definedName>
+    <definedName name="Bundesländer001" localSheetId="2">Indik_bis_einschl_01.02.!$G$2:$J$18</definedName>
+    <definedName name="Bundesländer001_1" localSheetId="1">Gesamt_bis_einschl_01.02.21!$D$3:$G$19</definedName>
+    <definedName name="Bundesländer001_1" localSheetId="2">Indik_bis_einschl_01.02.!$C$2:$F$18</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
 </workbook>
@@ -213,16 +208,16 @@
     <t>Anmerkung zu den Indikationen: Es können mehrere Indikationen je geimpfter Person vorliegen. In einigen Bundesländern werden nicht alle der in der Tabelle aufgeführten Indikationen einzeln ausgewiesen.</t>
   </si>
   <si>
-    <t>Durchgeführte Impfungen bundesweit und nach Bundesland bis einschließlich 31.01.21 (Gesamt_bis_einschl_31.01.21)</t>
-  </si>
-  <si>
-    <t>Anzahl Impfungen nach Indikation bis einschließlich 31.01.21 (Indik_bis_einschl_31.01.21)</t>
-  </si>
-  <si>
-    <t>Datenstand: 01.02.2021, 10:00 Uhr</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Die kumulative Zahl der Impfungen umfasst alle Impfungen, die bis einschließlich 31.01.21 durchgeführt und bis zum 01.02.21, 10:00 Uhr, dem RKI gemeldet wurden. Nachmeldungen aus zurückliegenden Tagen sind in der kumulativen Zahl der Impfungen enthalten. </t>
+    <t>Datenstand: 02.02.2021, 10:00 Uhr</t>
+  </si>
+  <si>
+    <t>Durchgeführte Impfungen bundesweit und nach Bundesland bis einschließlich 01.02.21 (Gesamt_bis_einschl_01.02.21)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Die kumulative Zahl der Impfungen umfasst alle Impfungen, die bis einschließlich 01.02.21 durchgeführt und bis zum 02.02.21, 10:00 Uhr, dem RKI gemeldet wurden. Nachmeldungen aus zurückliegenden Tagen sind in der kumulativen Zahl der Impfungen enthalten. </t>
+  </si>
+  <si>
+    <t>Anzahl Impfungen nach Indikation bis einschließlich 01.02.21 (Indik_bis_einschl_01.02.21)</t>
   </si>
 </sst>
 </file>
@@ -797,7 +792,7 @@
 </file>
 
 <file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="Bundesländer001" fillFormulas="1" connectionId="1" xr16:uid="{8C6643A4-82D3-4F11-ADE7-BA4132573BCB}" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0">
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="Bundesländer001_1" fillFormulas="1" connectionId="2" xr16:uid="{85D177FD-4909-4AAF-B663-F45CEC25E8F5}" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0">
   <queryTableRefresh preserveSortFilterLayout="0" nextId="13">
     <queryTableFields count="4">
       <queryTableField id="5" name="Fälle in den letzten 7 Tagen"/>
@@ -818,7 +813,7 @@
 </file>
 
 <file path=xl/queryTables/queryTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="Bundesländer001_1" fillFormulas="1" connectionId="2" xr16:uid="{85D177FD-4909-4AAF-B663-F45CEC25E8F5}" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0">
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="Bundesländer001" fillFormulas="1" connectionId="1" xr16:uid="{8C6643A4-82D3-4F11-ADE7-BA4132573BCB}" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0">
   <queryTableRefresh preserveSortFilterLayout="0" nextId="13">
     <queryTableFields count="4">
       <queryTableField id="5" name="Fälle in den letzten 7 Tagen"/>
@@ -1161,7 +1156,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5241AA5B-8CBB-47B1-9317-352256D0A517}">
   <dimension ref="A1:C22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1181,7 +1178,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="41" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B3" s="7"/>
       <c r="C3" s="8"/>
@@ -1193,12 +1190,12 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="45" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="44" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -1219,7 +1216,7 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="45" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -1282,7 +1279,7 @@
   <dimension ref="A1:K27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:A3"/>
+      <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1366,28 +1363,28 @@
         <v>1</v>
       </c>
       <c r="C4" s="35">
-        <v>295508</v>
+        <v>308205</v>
       </c>
       <c r="D4" s="17">
-        <v>230919</v>
+        <v>238397</v>
       </c>
       <c r="E4" s="17">
-        <v>225789</v>
+        <v>232766</v>
       </c>
       <c r="F4" s="17">
-        <v>5130</v>
+        <v>5631</v>
       </c>
       <c r="G4" s="17">
-        <v>5855</v>
+        <v>7169</v>
       </c>
       <c r="H4" s="34">
-        <v>2.0802775108703346</v>
+        <v>2.1476444890154349</v>
       </c>
       <c r="I4" s="30">
-        <v>64589</v>
+        <v>69808</v>
       </c>
       <c r="J4" s="21">
-        <v>4059</v>
+        <v>5175</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
@@ -1398,28 +1395,28 @@
         <v>0</v>
       </c>
       <c r="C5" s="36">
-        <v>440401</v>
+        <v>463122</v>
       </c>
       <c r="D5" s="22">
-        <v>324861</v>
+        <v>331825</v>
       </c>
       <c r="E5" s="22">
-        <v>315185</v>
+        <v>321822</v>
       </c>
       <c r="F5" s="22">
-        <v>9676</v>
+        <v>10003</v>
       </c>
       <c r="G5" s="23">
-        <v>3919</v>
+        <v>6964</v>
       </c>
       <c r="H5" s="24">
-        <v>2.4751810264845688</v>
+        <v>2.5282411373271709</v>
       </c>
       <c r="I5" s="31">
-        <v>115540</v>
+        <v>131297</v>
       </c>
       <c r="J5" s="25">
-        <v>9353</v>
+        <v>15757</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
@@ -1430,28 +1427,28 @@
         <v>3</v>
       </c>
       <c r="C6" s="35">
-        <v>130266</v>
+        <v>134937</v>
       </c>
       <c r="D6" s="17">
-        <v>97440</v>
+        <v>100283</v>
       </c>
       <c r="E6" s="17">
-        <v>94822</v>
+        <v>97521</v>
       </c>
       <c r="F6" s="17">
-        <v>2618</v>
+        <v>2762</v>
       </c>
       <c r="G6" s="18">
-        <v>2769</v>
+        <v>2843</v>
       </c>
       <c r="H6" s="19">
-        <v>2.655409156201773</v>
+        <v>2.7328858416603286</v>
       </c>
       <c r="I6" s="30">
-        <v>32826</v>
+        <v>34654</v>
       </c>
       <c r="J6" s="21">
-        <v>1049</v>
+        <v>1828</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
@@ -1462,28 +1459,28 @@
         <v>2</v>
       </c>
       <c r="C7" s="36">
-        <v>86804</v>
+        <v>89924</v>
       </c>
       <c r="D7" s="22">
-        <v>73844</v>
+        <v>75399</v>
       </c>
       <c r="E7" s="22">
-        <v>73154</v>
+        <v>74491</v>
       </c>
       <c r="F7" s="22">
-        <v>690</v>
+        <v>908</v>
       </c>
       <c r="G7" s="23">
-        <v>0</v>
+        <v>1444</v>
       </c>
       <c r="H7" s="24">
-        <v>2.9281178860482977</v>
+        <v>2.9897779168267644</v>
       </c>
       <c r="I7" s="31">
-        <v>12960</v>
+        <v>14525</v>
       </c>
       <c r="J7" s="25">
-        <v>0</v>
+        <v>1571</v>
       </c>
       <c r="K7" s="42"/>
     </row>
@@ -1495,28 +1492,28 @@
         <v>4</v>
       </c>
       <c r="C8" s="35">
-        <v>24656</v>
+        <v>25682</v>
       </c>
       <c r="D8" s="17">
-        <v>19415</v>
+        <v>19764</v>
       </c>
       <c r="E8" s="17">
-        <v>18158</v>
+        <v>18507</v>
       </c>
       <c r="F8" s="17">
         <v>1257</v>
       </c>
       <c r="G8" s="18">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="H8" s="19">
-        <v>2.85010907190525</v>
+        <v>2.9013420395125089</v>
       </c>
       <c r="I8" s="30">
-        <v>5241</v>
+        <v>5918</v>
       </c>
       <c r="J8" s="21">
-        <v>462</v>
+        <v>677</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
@@ -1527,28 +1524,28 @@
         <v>5</v>
       </c>
       <c r="C9" s="36">
-        <v>57119</v>
+        <v>59820</v>
       </c>
       <c r="D9" s="22">
-        <v>46374</v>
+        <v>47605</v>
       </c>
       <c r="E9" s="22">
-        <v>45854</v>
+        <v>47085</v>
       </c>
       <c r="F9" s="22">
         <v>520</v>
       </c>
       <c r="G9" s="23">
-        <v>1082</v>
+        <v>1231</v>
       </c>
       <c r="H9" s="24">
-        <v>2.5104303525288629</v>
+        <v>2.5770698437084687</v>
       </c>
       <c r="I9" s="31">
-        <v>10745</v>
+        <v>12215</v>
       </c>
       <c r="J9" s="25">
-        <v>1177</v>
+        <v>1348</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
@@ -1559,28 +1556,28 @@
         <v>15</v>
       </c>
       <c r="C10" s="35">
-        <v>176896</v>
+        <v>184555</v>
       </c>
       <c r="D10" s="17">
-        <v>130763</v>
+        <v>135211</v>
       </c>
       <c r="E10" s="17">
-        <v>130763</v>
+        <v>135211</v>
       </c>
       <c r="F10" s="17">
         <v>0</v>
       </c>
       <c r="G10" s="18">
-        <v>4179</v>
+        <v>4448</v>
       </c>
       <c r="H10" s="19">
-        <v>2.0795377921400493</v>
+        <v>2.1502748056640502</v>
       </c>
       <c r="I10" s="30">
-        <v>46133</v>
+        <v>49344</v>
       </c>
       <c r="J10" s="21">
-        <v>3119</v>
+        <v>3211</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
@@ -1591,28 +1588,28 @@
         <v>6</v>
       </c>
       <c r="C11" s="37">
-        <v>71322</v>
+        <v>73909</v>
       </c>
       <c r="D11" s="22">
-        <v>56289</v>
+        <v>57239</v>
       </c>
       <c r="E11" s="22">
-        <v>54624</v>
+        <v>55508</v>
       </c>
       <c r="F11" s="22">
-        <v>1665</v>
+        <v>1731</v>
       </c>
       <c r="G11" s="23">
-        <v>0</v>
+        <v>802</v>
       </c>
       <c r="H11" s="24">
-        <v>3.5002593061043266</v>
+        <v>3.5593338382651241</v>
       </c>
       <c r="I11" s="31">
-        <v>15033</v>
+        <v>16670</v>
       </c>
       <c r="J11" s="25">
-        <v>0</v>
+        <v>1078</v>
       </c>
       <c r="K11" s="9"/>
     </row>
@@ -1624,28 +1621,28 @@
         <v>7</v>
       </c>
       <c r="C12" s="35">
-        <v>196370</v>
+        <v>208258</v>
       </c>
       <c r="D12" s="17">
-        <v>151609</v>
+        <v>155283</v>
       </c>
       <c r="E12" s="17">
-        <v>149537</v>
+        <v>153211</v>
       </c>
       <c r="F12" s="17">
         <v>2072</v>
       </c>
       <c r="G12" s="18">
-        <v>1783</v>
+        <v>3093</v>
       </c>
       <c r="H12" s="19">
-        <v>1.8966279056966517</v>
+        <v>1.942589629113662</v>
       </c>
       <c r="I12" s="30">
-        <v>44761</v>
+        <v>52975</v>
       </c>
       <c r="J12" s="21">
-        <v>584</v>
+        <v>7742</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
@@ -1656,28 +1653,28 @@
         <v>8</v>
       </c>
       <c r="C13" s="36">
-        <v>456593</v>
+        <v>482207</v>
       </c>
       <c r="D13" s="22">
-        <v>357397</v>
+        <v>363713</v>
       </c>
       <c r="E13" s="22">
-        <v>352532</v>
+        <v>358848</v>
       </c>
       <c r="F13" s="22">
         <v>4865</v>
       </c>
       <c r="G13" s="23">
-        <v>6110</v>
+        <v>1732</v>
       </c>
       <c r="H13" s="24">
-        <v>1.9913779409079544</v>
+        <v>2.0265700188346707</v>
       </c>
       <c r="I13" s="31">
-        <v>99196</v>
+        <v>118494</v>
       </c>
       <c r="J13" s="25">
-        <v>4492</v>
+        <v>8300</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
@@ -1688,28 +1685,28 @@
         <v>12</v>
       </c>
       <c r="C14" s="35">
-        <v>159127</v>
+        <v>166064</v>
       </c>
       <c r="D14" s="17">
-        <v>141500</v>
+        <v>142618</v>
       </c>
       <c r="E14" s="17">
-        <v>137695</v>
+        <v>138813</v>
       </c>
       <c r="F14" s="17">
         <v>3805</v>
       </c>
       <c r="G14" s="18">
-        <v>541</v>
+        <v>71</v>
       </c>
       <c r="H14" s="19">
-        <v>3.4563593714848642</v>
+        <v>3.4836682745047942</v>
       </c>
       <c r="I14" s="30">
-        <v>17627</v>
+        <v>23446</v>
       </c>
       <c r="J14" s="21">
-        <v>803</v>
+        <v>5748</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
@@ -1720,28 +1717,28 @@
         <v>13</v>
       </c>
       <c r="C15" s="36">
-        <v>30425</v>
+        <v>31961</v>
       </c>
       <c r="D15" s="22">
-        <v>21589</v>
+        <v>22252</v>
       </c>
       <c r="E15" s="22">
-        <v>20751</v>
+        <v>21282</v>
       </c>
       <c r="F15" s="22">
-        <v>838</v>
+        <v>970</v>
       </c>
       <c r="G15" s="23">
-        <v>0</v>
+        <v>663</v>
       </c>
       <c r="H15" s="24">
-        <v>2.1875858127627579</v>
+        <v>2.2547667564776921</v>
       </c>
       <c r="I15" s="31">
-        <v>8836</v>
+        <v>9709</v>
       </c>
       <c r="J15" s="25">
-        <v>0</v>
+        <v>873</v>
       </c>
       <c r="K15" s="42"/>
     </row>
@@ -1753,28 +1750,28 @@
         <v>9</v>
       </c>
       <c r="C16" s="35">
-        <v>105841</v>
+        <v>112217</v>
       </c>
       <c r="D16" s="17">
-        <v>89519</v>
+        <v>92418</v>
       </c>
       <c r="E16" s="17">
-        <v>88476</v>
+        <v>91320</v>
       </c>
       <c r="F16" s="17">
-        <v>1043</v>
+        <v>1098</v>
       </c>
       <c r="G16" s="18">
-        <v>2575</v>
+        <v>2899</v>
       </c>
       <c r="H16" s="19">
-        <v>2.1984193895290511</v>
+        <v>2.2696134132585915</v>
       </c>
       <c r="I16" s="30">
-        <v>16322</v>
+        <v>19799</v>
       </c>
       <c r="J16" s="21">
-        <v>1247</v>
+        <v>3477</v>
       </c>
       <c r="K16" s="42"/>
     </row>
@@ -1786,28 +1783,28 @@
         <v>10</v>
       </c>
       <c r="C17" s="36">
-        <v>70505</v>
+        <v>73687</v>
       </c>
       <c r="D17" s="22">
-        <v>50324</v>
+        <v>51791</v>
       </c>
       <c r="E17" s="22">
-        <v>49749</v>
+        <v>51183</v>
       </c>
       <c r="F17" s="22">
-        <v>575</v>
+        <v>608</v>
       </c>
       <c r="G17" s="23">
-        <v>314</v>
+        <v>1467</v>
       </c>
       <c r="H17" s="24">
-        <v>2.2928928704536484</v>
+        <v>2.35973322179606</v>
       </c>
       <c r="I17" s="31">
-        <v>20181</v>
+        <v>21896</v>
       </c>
       <c r="J17" s="25">
-        <v>433</v>
+        <v>1715</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
@@ -1818,28 +1815,28 @@
         <v>11</v>
       </c>
       <c r="C18" s="35">
-        <v>103043</v>
+        <v>106077</v>
       </c>
       <c r="D18" s="17">
-        <v>90151</v>
+        <v>91476</v>
       </c>
       <c r="E18" s="17">
-        <v>89753</v>
+        <v>91014</v>
       </c>
       <c r="F18" s="17">
-        <v>398</v>
+        <v>462</v>
       </c>
       <c r="G18" s="18">
-        <v>67</v>
+        <v>1325</v>
       </c>
       <c r="H18" s="19">
-        <v>3.1046159599941179</v>
+        <v>3.1502462485876133</v>
       </c>
       <c r="I18" s="30">
-        <v>12892</v>
+        <v>14601</v>
       </c>
       <c r="J18" s="21">
-        <v>1229</v>
+        <v>1709</v>
       </c>
       <c r="K18" s="42"/>
     </row>
@@ -1851,28 +1848,28 @@
         <v>14</v>
       </c>
       <c r="C19" s="36">
-        <v>63042</v>
+        <v>66372</v>
       </c>
       <c r="D19" s="22">
-        <v>53362</v>
+        <v>54937</v>
       </c>
       <c r="E19" s="22">
-        <v>53362</v>
+        <v>54937</v>
       </c>
       <c r="F19" s="22">
         <v>0</v>
       </c>
       <c r="G19" s="23">
-        <v>827</v>
+        <v>1575</v>
       </c>
       <c r="H19" s="24">
-        <v>2.5012913792117475</v>
+        <v>2.5751179584677444</v>
       </c>
       <c r="I19" s="31">
-        <v>9680</v>
+        <v>11435</v>
       </c>
       <c r="J19" s="25">
-        <v>0</v>
+        <v>1653</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
@@ -1882,35 +1879,35 @@
       </c>
       <c r="C20" s="38">
         <f>D20+I20</f>
-        <v>2467918</v>
+        <v>2586997</v>
       </c>
       <c r="D20" s="6">
         <f>SUM(D4:D19)</f>
-        <v>1935356</v>
+        <v>1980211</v>
       </c>
       <c r="E20" s="6">
         <f>SUM(E4:E19)</f>
-        <v>1900204</v>
+        <v>1943519</v>
       </c>
       <c r="F20" s="6">
         <f>SUM(F4:F19)</f>
-        <v>35152</v>
+        <v>36692</v>
       </c>
       <c r="G20" s="6">
         <f>SUM(G4:G19)</f>
-        <v>30370</v>
+        <v>38074</v>
       </c>
       <c r="H20" s="10">
         <f>D20/83166711*100</f>
-        <v>2.3270801222378505</v>
+        <v>2.3810139612230188</v>
       </c>
       <c r="I20" s="29">
         <f>SUM(I4:I19)</f>
-        <v>532562</v>
+        <v>606786</v>
       </c>
       <c r="J20" s="32">
         <f>SUM(J4:J19)</f>
-        <v>28007</v>
+        <v>61862</v>
       </c>
     </row>
     <row r="22" spans="1:11" s="42" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1951,7 +1948,7 @@
   <dimension ref="A1:K27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:A2"/>
+      <selection activeCell="K9" sqref="K9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2024,28 +2021,28 @@
         <v>1</v>
       </c>
       <c r="C3" s="20">
-        <v>134496</v>
+        <v>138565</v>
       </c>
       <c r="D3" s="18">
-        <v>76908</v>
+        <v>79455</v>
       </c>
       <c r="E3" s="18">
-        <v>7687</v>
+        <v>7937</v>
       </c>
       <c r="F3" s="21">
-        <v>43386</v>
+        <v>45472</v>
       </c>
       <c r="G3" s="20">
-        <v>37527</v>
+        <v>40954</v>
       </c>
       <c r="H3" s="18">
-        <v>21280</v>
+        <v>22823</v>
       </c>
       <c r="I3" s="18">
-        <v>1199</v>
+        <v>1276</v>
       </c>
       <c r="J3" s="21">
-        <v>10585</v>
+        <v>11575</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
@@ -2056,28 +2053,28 @@
         <v>0</v>
       </c>
       <c r="C4" s="26">
-        <v>117652</v>
+        <v>120160</v>
       </c>
       <c r="D4" s="23">
-        <v>165208</v>
+        <v>168487</v>
       </c>
       <c r="E4" s="23">
-        <v>6881</v>
+        <v>7107</v>
       </c>
       <c r="F4" s="25">
-        <v>88536</v>
+        <v>89551</v>
       </c>
       <c r="G4" s="26">
-        <v>40199</v>
+        <v>44542</v>
       </c>
       <c r="H4" s="23">
-        <v>58184</v>
+        <v>67217</v>
       </c>
       <c r="I4" s="23">
-        <v>1535</v>
+        <v>1710</v>
       </c>
       <c r="J4" s="25">
-        <v>40686</v>
+        <v>44554</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
@@ -2088,28 +2085,28 @@
         <v>3</v>
       </c>
       <c r="C5" s="20">
-        <v>70467</v>
+        <v>73051</v>
       </c>
       <c r="D5" s="18">
-        <v>24252</v>
+        <v>24486</v>
       </c>
       <c r="E5" s="18">
         <v>108</v>
       </c>
       <c r="F5" s="21">
-        <v>33012</v>
+        <v>33152</v>
       </c>
       <c r="G5" s="20">
-        <v>22515</v>
+        <v>24060</v>
       </c>
       <c r="H5" s="18">
-        <v>8513</v>
+        <v>8866</v>
       </c>
       <c r="I5" s="18">
         <v>28</v>
       </c>
       <c r="J5" s="21">
-        <v>20815</v>
+        <v>21594</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
@@ -2120,28 +2117,28 @@
         <v>2</v>
       </c>
       <c r="C6" s="26">
-        <v>31554</v>
+        <v>32798</v>
       </c>
       <c r="D6" s="23">
-        <v>38952</v>
+        <v>39427</v>
       </c>
       <c r="E6" s="23">
-        <v>1068</v>
+        <v>1093</v>
       </c>
       <c r="F6" s="25">
-        <v>16268</v>
+        <v>17209</v>
       </c>
       <c r="G6" s="26">
-        <v>832</v>
+        <v>1822</v>
       </c>
       <c r="H6" s="23">
-        <v>12124</v>
+        <v>12653</v>
       </c>
       <c r="I6" s="23">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="J6" s="25">
-        <v>754</v>
+        <v>1385</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
@@ -2152,28 +2149,28 @@
         <v>4</v>
       </c>
       <c r="C7" s="20">
-        <v>8402</v>
+        <v>8606</v>
       </c>
       <c r="D7" s="18">
-        <v>7996</v>
+        <v>8081</v>
       </c>
       <c r="E7" s="18">
-        <v>139</v>
+        <v>147</v>
       </c>
       <c r="F7" s="21">
-        <v>6764</v>
+        <v>6825</v>
       </c>
       <c r="G7" s="20">
-        <v>1875</v>
+        <v>2102</v>
       </c>
       <c r="H7" s="18">
-        <v>2200</v>
+        <v>2549</v>
       </c>
       <c r="I7" s="18">
         <v>23</v>
       </c>
       <c r="J7" s="21">
-        <v>2051</v>
+        <v>2366</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
@@ -2184,28 +2181,28 @@
         <v>5</v>
       </c>
       <c r="C8" s="26">
-        <v>17916</v>
+        <v>18558</v>
       </c>
       <c r="D8" s="23">
-        <v>22785</v>
+        <v>23337</v>
       </c>
       <c r="E8" s="23">
-        <v>1840</v>
+        <v>1842</v>
       </c>
       <c r="F8" s="25">
-        <v>11393</v>
+        <v>11701</v>
       </c>
       <c r="G8" s="26">
-        <v>3419</v>
+        <v>3960</v>
       </c>
       <c r="H8" s="23">
-        <v>6497</v>
+        <v>7341</v>
       </c>
       <c r="I8" s="23">
-        <v>129</v>
+        <v>144</v>
       </c>
       <c r="J8" s="25">
-        <v>2655</v>
+        <v>2928</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
@@ -2216,28 +2213,28 @@
         <v>15</v>
       </c>
       <c r="C9" s="20">
-        <v>54562</v>
+        <v>57107</v>
       </c>
       <c r="D9" s="18">
-        <v>57843</v>
+        <v>59310</v>
       </c>
       <c r="E9" s="18">
-        <v>4993</v>
+        <v>5129</v>
       </c>
       <c r="F9" s="21">
-        <v>36796</v>
+        <v>37338</v>
       </c>
       <c r="G9" s="20">
-        <v>10964</v>
+        <v>11902</v>
       </c>
       <c r="H9" s="18">
-        <v>25521</v>
+        <v>27146</v>
       </c>
       <c r="I9" s="18">
-        <v>3595</v>
+        <v>3715</v>
       </c>
       <c r="J9" s="21">
-        <v>16941</v>
+        <v>18573</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
@@ -2248,28 +2245,28 @@
         <v>6</v>
       </c>
       <c r="C10" s="26">
-        <v>10559</v>
+        <v>10839</v>
       </c>
       <c r="D10" s="23">
-        <v>24777</v>
+        <v>25234</v>
       </c>
       <c r="E10" s="23">
-        <v>1205</v>
+        <v>1251</v>
       </c>
       <c r="F10" s="25">
-        <v>20401</v>
+        <v>20627</v>
       </c>
       <c r="G10" s="26">
-        <v>1318</v>
+        <v>1430</v>
       </c>
       <c r="H10" s="23">
-        <v>987</v>
+        <v>9656</v>
       </c>
       <c r="I10" s="23">
-        <v>0</v>
+        <v>151</v>
       </c>
       <c r="J10" s="25">
-        <v>0</v>
+        <v>5757</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
@@ -2280,28 +2277,28 @@
         <v>7</v>
       </c>
       <c r="C11" s="20">
-        <v>29442</v>
+        <v>30938</v>
       </c>
       <c r="D11" s="18">
-        <v>83378</v>
+        <v>85046</v>
       </c>
       <c r="E11" s="18">
-        <v>24136</v>
+        <v>24510</v>
       </c>
       <c r="F11" s="21">
-        <v>66073</v>
+        <v>67500</v>
       </c>
       <c r="G11" s="20">
-        <v>9570</v>
+        <v>11011</v>
       </c>
       <c r="H11" s="18">
-        <v>22228</v>
+        <v>26979</v>
       </c>
       <c r="I11" s="18">
-        <v>8240</v>
+        <v>9215</v>
       </c>
       <c r="J11" s="21">
-        <v>21258</v>
+        <v>24664</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
@@ -2312,28 +2309,28 @@
         <v>8</v>
       </c>
       <c r="C12" s="26">
-        <v>53909</v>
+        <v>54821</v>
       </c>
       <c r="D12" s="23">
-        <v>195794</v>
+        <v>200072</v>
       </c>
       <c r="E12" s="23">
-        <v>10173</v>
+        <v>10565</v>
       </c>
       <c r="F12" s="25">
-        <v>154051</v>
+        <v>155896</v>
       </c>
       <c r="G12" s="26">
-        <v>19176</v>
+        <v>22887</v>
       </c>
       <c r="H12" s="23">
-        <v>49280</v>
+        <v>59566</v>
       </c>
       <c r="I12" s="23">
-        <v>3477</v>
+        <v>4339</v>
       </c>
       <c r="J12" s="25">
-        <v>48473</v>
+        <v>56858</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
@@ -2344,28 +2341,28 @@
         <v>12</v>
       </c>
       <c r="C13" s="20">
-        <v>52078</v>
+        <v>52120</v>
       </c>
       <c r="D13" s="18">
-        <v>56599</v>
+        <v>57179</v>
       </c>
       <c r="E13" s="18">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="F13" s="21">
-        <v>32738</v>
+        <v>33233</v>
       </c>
       <c r="G13" s="20">
-        <v>4330</v>
+        <v>7757</v>
       </c>
       <c r="H13" s="18">
-        <v>9344</v>
+        <v>11226</v>
       </c>
       <c r="I13" s="18">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="J13" s="21">
-        <v>3938</v>
+        <v>4441</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
@@ -2376,28 +2373,28 @@
         <v>13</v>
       </c>
       <c r="C14" s="26">
-        <v>14253</v>
+        <v>14568</v>
       </c>
       <c r="D14" s="23">
-        <v>5728</v>
+        <v>6072</v>
       </c>
       <c r="E14" s="23">
         <v>1</v>
       </c>
       <c r="F14" s="25">
-        <v>5717</v>
+        <v>5726</v>
       </c>
       <c r="G14" s="26">
-        <v>6741</v>
+        <v>7426</v>
       </c>
       <c r="H14" s="23">
-        <v>1130</v>
+        <v>1250</v>
       </c>
       <c r="I14" s="23">
         <v>0</v>
       </c>
       <c r="J14" s="25">
-        <v>3029</v>
+        <v>3301</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
@@ -2408,28 +2405,28 @@
         <v>9</v>
       </c>
       <c r="C15" s="20">
-        <v>11599</v>
+        <v>12983</v>
       </c>
       <c r="D15" s="18">
-        <v>59494</v>
+        <v>60467</v>
       </c>
       <c r="E15" s="18">
-        <v>600</v>
+        <v>950</v>
       </c>
       <c r="F15" s="21">
-        <v>23358</v>
+        <v>23848</v>
       </c>
       <c r="G15" s="20">
-        <v>1170</v>
+        <v>1435</v>
       </c>
       <c r="H15" s="18">
-        <v>12004</v>
+        <v>14210</v>
       </c>
       <c r="I15" s="18">
-        <v>241</v>
+        <v>408</v>
       </c>
       <c r="J15" s="21">
-        <v>2641</v>
+        <v>2783</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
@@ -2440,28 +2437,28 @@
         <v>10</v>
       </c>
       <c r="C16" s="26">
-        <v>16822</v>
+        <v>17502</v>
       </c>
       <c r="D16" s="23">
-        <v>25188</v>
+        <v>25920</v>
       </c>
       <c r="E16" s="23">
-        <v>2118</v>
+        <v>2162</v>
       </c>
       <c r="F16" s="25">
-        <v>18119</v>
+        <v>18362</v>
       </c>
       <c r="G16" s="26">
-        <v>6404</v>
+        <v>6831</v>
       </c>
       <c r="H16" s="23">
-        <v>10135</v>
+        <v>11186</v>
       </c>
       <c r="I16" s="23">
-        <v>1538</v>
+        <v>1556</v>
       </c>
       <c r="J16" s="25">
-        <v>9041</v>
+        <v>9497</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
@@ -2472,28 +2469,28 @@
         <v>11</v>
       </c>
       <c r="C17" s="20">
-        <v>26576</v>
+        <v>26903</v>
       </c>
       <c r="D17" s="18">
-        <v>27061</v>
+        <v>27328</v>
       </c>
       <c r="E17" s="18">
-        <v>6128</v>
+        <v>6280</v>
       </c>
       <c r="F17" s="21">
-        <v>23406</v>
+        <v>24445</v>
       </c>
       <c r="G17" s="20">
-        <v>7611</v>
+        <v>8767</v>
       </c>
       <c r="H17" s="18">
-        <v>2953</v>
+        <v>3433</v>
       </c>
       <c r="I17" s="18">
-        <v>1428</v>
+        <v>1461</v>
       </c>
       <c r="J17" s="21">
-        <v>2402</v>
+        <v>2742</v>
       </c>
       <c r="K17" s="42"/>
     </row>
@@ -2505,28 +2502,28 @@
         <v>14</v>
       </c>
       <c r="C18" s="23">
-        <v>19706</v>
+        <v>20690</v>
       </c>
       <c r="D18" s="23">
-        <v>10611</v>
+        <v>27111</v>
       </c>
       <c r="E18" s="23">
-        <v>2119</v>
+        <v>2225</v>
       </c>
       <c r="F18" s="25">
-        <v>6788</v>
+        <v>6936</v>
       </c>
       <c r="G18" s="23">
-        <v>1050</v>
+        <v>1592</v>
       </c>
       <c r="H18" s="23">
-        <v>7981</v>
+        <v>8994</v>
       </c>
       <c r="I18" s="23">
-        <v>65</v>
+        <v>159</v>
       </c>
       <c r="J18" s="25">
-        <v>667</v>
+        <v>1122</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
@@ -2536,35 +2533,35 @@
       </c>
       <c r="C19" s="4">
         <f>SUM(C3:C18)</f>
-        <v>669993</v>
+        <v>690209</v>
       </c>
       <c r="D19" s="5">
         <f t="shared" ref="D19:J19" si="0">SUM(D3:D18)</f>
-        <v>882574</v>
+        <v>917012</v>
       </c>
       <c r="E19" s="5">
         <f t="shared" si="0"/>
-        <v>69281</v>
+        <v>71393</v>
       </c>
       <c r="F19" s="11">
         <f t="shared" si="0"/>
-        <v>586806</v>
+        <v>597821</v>
       </c>
       <c r="G19" s="4">
         <f t="shared" si="0"/>
-        <v>174701</v>
+        <v>198478</v>
       </c>
       <c r="H19" s="5">
         <f t="shared" si="0"/>
-        <v>250361</v>
+        <v>295095</v>
       </c>
       <c r="I19" s="5">
         <f t="shared" si="0"/>
-        <v>21514</v>
+        <v>24218</v>
       </c>
       <c r="J19" s="11">
         <f t="shared" si="0"/>
-        <v>185936</v>
+        <v>214140</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
@@ -2602,9 +2599,11 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{926B42D2-7956-44E7-BD5B-5AF896796AC0}">
-  <dimension ref="A1:D39"/>
+  <dimension ref="A1:D45"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="G40" sqref="G40"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2675,13 +2674,13 @@
         <v>44195</v>
       </c>
       <c r="B5" s="43">
-        <v>57454</v>
+        <v>57632</v>
       </c>
       <c r="C5" s="47">
         <v>0</v>
       </c>
       <c r="D5" s="47">
-        <v>57454</v>
+        <v>57632</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -2717,13 +2716,13 @@
         <v>44198</v>
       </c>
       <c r="B8" s="43">
-        <v>50377</v>
+        <v>50567</v>
       </c>
       <c r="C8" s="47">
         <v>0</v>
       </c>
       <c r="D8" s="47">
-        <v>50377</v>
+        <v>50567</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -2731,13 +2730,13 @@
         <v>44199</v>
       </c>
       <c r="B9" s="43">
-        <v>24849</v>
+        <v>24979</v>
       </c>
       <c r="C9" s="47">
         <v>0</v>
       </c>
       <c r="D9" s="47">
-        <v>24849</v>
+        <v>24979</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -2745,13 +2744,13 @@
         <v>44200</v>
       </c>
       <c r="B10" s="43">
-        <v>48667</v>
+        <v>48732</v>
       </c>
       <c r="C10" s="47">
         <v>0</v>
       </c>
       <c r="D10" s="47">
-        <v>48667</v>
+        <v>48732</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -2759,13 +2758,13 @@
         <v>44201</v>
       </c>
       <c r="B11" s="43">
-        <v>51974</v>
+        <v>52057</v>
       </c>
       <c r="C11" s="47">
         <v>0</v>
       </c>
       <c r="D11" s="47">
-        <v>51974</v>
+        <v>52057</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -2773,13 +2772,13 @@
         <v>44202</v>
       </c>
       <c r="B12" s="43">
-        <v>58215</v>
+        <v>58408</v>
       </c>
       <c r="C12" s="47">
         <v>0</v>
       </c>
       <c r="D12" s="47">
-        <v>58215</v>
+        <v>58408</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -2787,13 +2786,13 @@
         <v>44203</v>
       </c>
       <c r="B13" s="43">
-        <v>58030</v>
+        <v>58596</v>
       </c>
       <c r="C13" s="47">
         <v>0</v>
       </c>
       <c r="D13" s="47">
-        <v>58030</v>
+        <v>58596</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -2801,13 +2800,13 @@
         <v>44204</v>
       </c>
       <c r="B14" s="43">
-        <v>59007</v>
+        <v>59476</v>
       </c>
       <c r="C14" s="47">
         <v>0</v>
       </c>
       <c r="D14" s="47">
-        <v>59007</v>
+        <v>59476</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -2815,13 +2814,13 @@
         <v>44205</v>
       </c>
       <c r="B15" s="43">
-        <v>56104</v>
+        <v>56498</v>
       </c>
       <c r="C15" s="47">
         <v>0</v>
       </c>
       <c r="D15" s="47">
-        <v>56104</v>
+        <v>56498</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -2829,13 +2828,13 @@
         <v>44206</v>
       </c>
       <c r="B16" s="43">
-        <v>33167</v>
+        <v>33216</v>
       </c>
       <c r="C16" s="47">
         <v>0</v>
       </c>
       <c r="D16" s="47">
-        <v>33167</v>
+        <v>33216</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -2843,13 +2842,13 @@
         <v>44207</v>
       </c>
       <c r="B17" s="43">
-        <v>65423</v>
+        <v>65469</v>
       </c>
       <c r="C17" s="47">
         <v>0</v>
       </c>
       <c r="D17" s="47">
-        <v>65423</v>
+        <v>65469</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -2857,13 +2856,13 @@
         <v>44208</v>
       </c>
       <c r="B18" s="43">
-        <v>81901</v>
+        <v>81839</v>
       </c>
       <c r="C18" s="47">
         <v>0</v>
       </c>
       <c r="D18" s="47">
-        <v>81901</v>
+        <v>81839</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
@@ -2871,13 +2870,13 @@
         <v>44209</v>
       </c>
       <c r="B19" s="43">
-        <v>98058</v>
+        <v>98160</v>
       </c>
       <c r="C19" s="47">
         <v>0</v>
       </c>
       <c r="D19" s="47">
-        <v>98058</v>
+        <v>98160</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -2885,13 +2884,13 @@
         <v>44210</v>
       </c>
       <c r="B20" s="43">
-        <v>100267</v>
+        <v>100336</v>
       </c>
       <c r="C20" s="47">
         <v>140</v>
       </c>
       <c r="D20" s="47">
-        <v>100407</v>
+        <v>100476</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
@@ -2899,13 +2898,13 @@
         <v>44211</v>
       </c>
       <c r="B21" s="43">
-        <v>92282</v>
+        <v>92366</v>
       </c>
       <c r="C21" s="47">
         <v>444</v>
       </c>
       <c r="D21" s="47">
-        <v>92726</v>
+        <v>92810</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
@@ -2913,13 +2912,13 @@
         <v>44212</v>
       </c>
       <c r="B22" s="43">
-        <v>56196</v>
+        <v>56385</v>
       </c>
       <c r="C22" s="47">
-        <v>505</v>
+        <v>506</v>
       </c>
       <c r="D22" s="47">
-        <v>56701</v>
+        <v>56891</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
@@ -2930,10 +2929,10 @@
         <v>31007</v>
       </c>
       <c r="C23" s="47">
-        <v>13536</v>
+        <v>13535</v>
       </c>
       <c r="D23" s="47">
-        <v>44543</v>
+        <v>44542</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
@@ -2941,13 +2940,13 @@
         <v>44214</v>
       </c>
       <c r="B24" s="43">
-        <v>57176</v>
+        <v>57435</v>
       </c>
       <c r="C24" s="47">
         <v>16476</v>
       </c>
       <c r="D24" s="47">
-        <v>73652</v>
+        <v>73911</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
@@ -2955,13 +2954,13 @@
         <v>44215</v>
       </c>
       <c r="B25" s="43">
-        <v>65361</v>
+        <v>66306</v>
       </c>
       <c r="C25" s="47">
         <v>27054</v>
       </c>
       <c r="D25" s="47">
-        <v>92415</v>
+        <v>93360</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
@@ -2969,13 +2968,13 @@
         <v>44216</v>
       </c>
       <c r="B26" s="43">
-        <v>76341</v>
+        <v>77014</v>
       </c>
       <c r="C26" s="47">
-        <v>49683</v>
+        <v>49687</v>
       </c>
       <c r="D26" s="47">
-        <v>126024</v>
+        <v>126701</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
@@ -2983,13 +2982,13 @@
         <v>44217</v>
       </c>
       <c r="B27" s="43">
-        <v>59586</v>
+        <v>59647</v>
       </c>
       <c r="C27" s="47">
-        <v>34136</v>
+        <v>34259</v>
       </c>
       <c r="D27" s="47">
-        <v>93722</v>
+        <v>93906</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
@@ -2997,13 +2996,13 @@
         <v>44218</v>
       </c>
       <c r="B28" s="43">
-        <v>83065</v>
+        <v>83090</v>
       </c>
       <c r="C28" s="47">
-        <v>30133</v>
+        <v>30245</v>
       </c>
       <c r="D28" s="47">
-        <v>113198</v>
+        <v>113335</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
@@ -3011,13 +3010,13 @@
         <v>44219</v>
       </c>
       <c r="B29" s="43">
-        <v>48020</v>
+        <v>48042</v>
       </c>
       <c r="C29" s="47">
-        <v>41550</v>
+        <v>42243</v>
       </c>
       <c r="D29" s="47">
-        <v>89570</v>
+        <v>90285</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
@@ -3025,13 +3024,13 @@
         <v>44220</v>
       </c>
       <c r="B30" s="43">
-        <v>37850</v>
+        <v>37869</v>
       </c>
       <c r="C30" s="47">
-        <v>27338</v>
+        <v>27518</v>
       </c>
       <c r="D30" s="47">
-        <v>65188</v>
+        <v>65387</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
@@ -3039,13 +3038,13 @@
         <v>44221</v>
       </c>
       <c r="B31" s="53">
-        <v>56923</v>
+        <v>57036</v>
       </c>
       <c r="C31" s="53">
-        <v>38587</v>
+        <v>38964</v>
       </c>
       <c r="D31" s="53">
-        <v>95510</v>
+        <v>96000</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
@@ -3053,13 +3052,13 @@
         <v>44222</v>
       </c>
       <c r="B32" s="53">
-        <v>52761</v>
+        <v>52782</v>
       </c>
       <c r="C32" s="53">
-        <v>47520</v>
+        <v>47766</v>
       </c>
       <c r="D32" s="53">
-        <v>100281</v>
+        <v>100548</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
@@ -3067,13 +3066,13 @@
         <v>44223</v>
       </c>
       <c r="B33" s="53">
-        <v>52924</v>
+        <v>53153</v>
       </c>
       <c r="C33" s="53">
-        <v>53035</v>
+        <v>55354</v>
       </c>
       <c r="D33" s="53">
-        <v>105959</v>
+        <v>108507</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
@@ -3081,13 +3080,13 @@
         <v>44224</v>
       </c>
       <c r="B34" s="53">
-        <v>51097</v>
+        <v>51278</v>
       </c>
       <c r="C34" s="53">
-        <v>46181</v>
+        <v>47082</v>
       </c>
       <c r="D34" s="53">
-        <v>97278</v>
+        <v>98360</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
@@ -3095,13 +3094,13 @@
         <v>44225</v>
       </c>
       <c r="B35" s="53">
-        <v>55051</v>
+        <v>55710</v>
       </c>
       <c r="C35" s="53">
-        <v>43228</v>
+        <v>47368</v>
       </c>
       <c r="D35" s="53">
-        <v>98279</v>
+        <v>103078</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
@@ -3109,13 +3108,13 @@
         <v>44226</v>
       </c>
       <c r="B36" s="53">
-        <v>36389</v>
+        <v>36795</v>
       </c>
       <c r="C36" s="53">
-        <v>35009</v>
+        <v>37611</v>
       </c>
       <c r="D36" s="53">
-        <v>71398</v>
+        <v>74406</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
@@ -3123,30 +3122,44 @@
         <v>44227</v>
       </c>
       <c r="B37" s="53">
-        <v>30370</v>
+        <v>30793</v>
       </c>
       <c r="C37" s="53">
-        <v>28007</v>
+        <v>28672</v>
       </c>
       <c r="D37" s="53">
-        <v>58377</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" s="16" t="s">
+        <v>59465</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" s="49">
+        <v>44228</v>
+      </c>
+      <c r="B38" s="53">
+        <v>38074</v>
+      </c>
+      <c r="C38" s="53">
+        <v>61862</v>
+      </c>
+      <c r="D38" s="53">
+        <v>99936</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="B39" s="15">
-        <f>SUM(B2:B37)</f>
-        <v>1935356</v>
-      </c>
-      <c r="C39" s="15">
-        <f>SUM(C2:C37)</f>
-        <v>532562</v>
-      </c>
-      <c r="D39" s="15">
-        <f>SUM(D2:D37)</f>
-        <v>2467918</v>
+      <c r="B45" s="15">
+        <f>SUM(B2:B43)</f>
+        <v>1980211</v>
+      </c>
+      <c r="C45" s="15">
+        <f t="shared" ref="C45:D45" si="0">SUM(C2:C43)</f>
+        <v>606786</v>
+      </c>
+      <c r="D45" s="15">
+        <f t="shared" si="0"/>
+        <v>2586997</v>
       </c>
     </row>
   </sheetData>

</xml_diff>